<commit_message>
Update regression test scripts and Add Detailsteps flag for log files.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.20.30.210_VerifyThatSiteIdUsedInRunCommandAction.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.20.30.210_VerifyThatSiteIdUsedInRunCommandAction.xlsx
@@ -3919,10 +3919,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"C:\run.bat"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>"C:\Nform\commandresult.txt"</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3935,6 +3931,10 @@
   </si>
   <si>
     <t>137</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"C:\runcommand.bat"</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4933,8 +4933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5141,7 +5141,7 @@
         <v>765</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C7" s="5">
         <v>6</v>
@@ -6084,10 +6084,10 @@
         <v>356</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>878</v>
+        <v>4</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>882</v>
       </c>
       <c r="I41" s="11"/>
       <c r="J41" s="5"/>
@@ -6114,7 +6114,7 @@
         <v>3</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I42" s="11"/>
       <c r="J42" s="5"/>
@@ -6141,7 +6141,7 @@
         <v>3</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I43" s="11"/>
       <c r="J43" s="5"/>
@@ -7066,7 +7066,7 @@
       <c r="F82" s="21"/>
       <c r="G82" s="21"/>
       <c r="H82" s="11" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I82" s="11" t="s">
         <v>858</v>
@@ -7092,7 +7092,7 @@
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
       <c r="H83" s="11" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I83" s="11" t="s">
         <v>859</v>
@@ -7818,7 +7818,7 @@
       <c r="F114" s="21"/>
       <c r="G114" s="21"/>
       <c r="H114" s="11" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I114" s="11" t="s">
         <v>867</v>
@@ -7844,7 +7844,7 @@
       <c r="F115" s="21"/>
       <c r="G115" s="21"/>
       <c r="H115" s="11" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I115" s="11" t="s">
         <v>868</v>

</xml_diff>